<commit_message>
Fixed formula in excel + added grahs
</commit_message>
<xml_diff>
--- a/beursbar_calculate_prices/simulation.xlsx
+++ b/beursbar_calculate_prices/simulation.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VS_project\beursbar_calc_prices\beursbar_calculate_prices\beursbar_calculate_prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Personal\Visual Studio 2017\Projects\beursbar_calc_prices\beursbar_calculate_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A57DC5F-C180-4EF9-9CBE-81212291F50F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{45767AAA-68F0-409E-98E0-A9D31519FA42}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>dranken</t>
   </si>
@@ -59,15 +60,24 @@
   <si>
     <t>prijs (opening was 2€)</t>
   </si>
+  <si>
+    <t>General formule:</t>
+  </si>
+  <si>
+    <t>new_price=old_price*(1+(delta times_sold/100))</t>
+  </si>
+  <si>
+    <t>spread</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +118,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -132,8 +148,2011 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.8923242082662372E-2"/>
+          <c:y val="1.1468146321413892E-2"/>
+          <c:w val="0.94926247987117551"/>
+          <c:h val="0.81386189889025895"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$47:$U$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$47:$U$47</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>00:05:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>00:10:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>00:15:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>00:20:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>00:25:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>00:30:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>00:35:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>00:40:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>00:45:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>00:50:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>00:55:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01:05:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>01:10:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>01:15:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>01:20:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>01:25:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>01:30:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>01:35:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>01:40:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$52:$U$52</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$52:$U$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B82E-4A2E-BDC2-8E56760CCD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$47:$U$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$47:$U$47</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>00:05:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>00:10:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>00:15:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>00:20:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>00:25:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>00:30:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>00:35:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>00:40:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>00:45:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>00:50:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>00:55:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01:05:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>01:10:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>01:15:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>01:20:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>01:25:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>01:30:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>01:35:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>01:40:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$53:$U$53</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$53:$U$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B82E-4A2E-BDC2-8E56760CCD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$47:$U$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$47:$U$47</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>00:05:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>00:10:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>00:15:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>00:20:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>00:25:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>00:30:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>00:35:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>00:40:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>00:45:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>00:50:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>00:55:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01:05:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>01:10:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>01:15:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>01:20:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>01:25:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>01:30:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>01:35:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>01:40:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$54:$U$54</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$54:$U$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B82E-4A2E-BDC2-8E56760CCD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$47:$U$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$47:$U$47</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>00:05:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>00:10:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>00:15:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>00:20:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>00:25:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>00:30:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>00:35:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>00:40:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>00:45:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>00:50:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>00:55:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01:05:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>01:10:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>01:15:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>01:20:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>01:25:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>01:30:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>01:35:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>01:40:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$55:$U$55</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$55:$U$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B82E-4A2E-BDC2-8E56760CCD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$47:$U$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$47:$U$47</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>00:05:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>00:10:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>00:15:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>00:20:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>00:25:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>00:30:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>00:35:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>00:40:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>00:45:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>00:50:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>00:55:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01:05:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>01:10:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>01:15:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>01:20:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>01:25:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>01:30:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>01:35:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>01:40:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$56:$U$56</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$56:$U$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B82E-4A2E-BDC2-8E56760CCD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$47:$U$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$47:$U$47</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>00:05:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>00:10:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>00:15:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>00:20:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>00:25:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>00:30:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>00:35:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>00:40:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>00:45:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>00:50:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>00:55:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01:05:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>01:10:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>01:15:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>01:20:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>01:25:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>01:30:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>01:35:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>01:40:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$57:$U$57</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$57:$U$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B82E-4A2E-BDC2-8E56760CCD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$47:$U$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$47:$U$47</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>00:05:00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>00:10:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>00:15:00</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>00:20:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>00:25:00</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>00:30:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>00:35:00</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>00:40:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>00:45:00</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>00:50:00</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>00:55:00</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>01:00:00</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01:05:00</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>01:10:00</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>01:15:00</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>01:20:00</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>01:25:00</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>01:30:00</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>01:35:00</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>01:40:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Blad1!$A$58:$U$58</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Blad1!$B$58:$U$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B82E-4A2E-BDC2-8E56760CCD62}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="463273928"/>
+        <c:axId val="400039744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="463273928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400039744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="400039744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="463273928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9315000" cy="6082500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D314C5-3D8C-4786-A239-1EAB453C0BE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -428,21 +2447,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8F9780-8CE8-4591-B954-E475CC11276C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +2469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -458,7 +2477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -466,7 +2485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -474,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -500,7 +2519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -508,7 +2527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -516,7 +2535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -524,34 +2543,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="34.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36" ht="34.5">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -616,7 +2635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36">
       <c r="A14">
         <v>-0.15</v>
       </c>
@@ -699,9 +2718,9 @@
         <f t="shared" si="0"/>
         <v>9.1198896669445473E-2</v>
       </c>
-      <c r="AJ14" s="3"/>
+      <c r="AJ14" s="2"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36">
       <c r="A15">
         <v>-0.14000000000000001</v>
       </c>
@@ -785,7 +2804,7 @@
         <v>0.11389392748450061</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36">
       <c r="A16">
         <v>-0.13</v>
       </c>
@@ -869,7 +2888,7 @@
         <v>0.14187170739891863</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21">
       <c r="A17">
         <v>-0.12</v>
       </c>
@@ -953,7 +2972,7 @@
         <v>0.17627907645043089</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21">
       <c r="A18">
         <v>-0.11</v>
       </c>
@@ -1037,7 +3056,7 @@
         <v>0.21849430512153944</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21">
       <c r="A19">
         <v>-0.1</v>
       </c>
@@ -1121,7 +3140,7 @@
         <v>0.27017034353459857</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21">
       <c r="A20">
         <v>-0.09</v>
       </c>
@@ -1205,7 +3224,7 @@
         <v>0.33328552318719978</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21">
       <c r="A21">
         <v>-0.08</v>
       </c>
@@ -1289,7 +3308,7 @@
         <v>0.41020288948434075</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21">
       <c r="A22">
         <v>-7.0000000000000007E-2</v>
       </c>
@@ -1373,7 +3392,7 @@
         <v>0.50373951325288469</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21">
       <c r="A23">
         <v>-0.06</v>
       </c>
@@ -1457,7 +3476,7 @@
         <v>0.61724732155630102</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21">
       <c r="A24">
         <v>-0.05</v>
       </c>
@@ -1541,7 +3560,7 @@
         <v>0.75470720507061428</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21">
       <c r="A25">
         <v>-0.04</v>
       </c>
@@ -1625,7 +3644,7 @@
         <v>0.92083840391543215</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21">
       <c r="A26">
         <v>-0.03</v>
       </c>
@@ -1709,7 +3728,7 @@
         <v>1.1212254493334992</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21">
       <c r="A27">
         <v>-0.02</v>
       </c>
@@ -1793,7 +3812,7 @@
         <v>1.3624652484797841</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21">
       <c r="A28">
         <v>-0.01</v>
       </c>
@@ -1877,7 +3896,7 @@
         <v>1.6523372476711731</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1942,7 +3961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21">
       <c r="A30">
         <v>0.01</v>
       </c>
@@ -2026,7 +4045,7 @@
         <v>2.4162179008870632</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21">
       <c r="A31">
         <v>0.02</v>
       </c>
@@ -2110,7 +4129,7 @@
         <v>2.9136223450555976</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21">
       <c r="A32">
         <v>0.03</v>
       </c>
@@ -2194,7 +4213,7 @@
         <v>3.5070121061542037</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21">
       <c r="A33">
         <v>0.04</v>
       </c>
@@ -2278,7 +4297,7 @@
         <v>4.2136983519873477</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21">
       <c r="A34">
         <v>0.05</v>
       </c>
@@ -2362,7 +4381,7 @@
         <v>5.0539003907512807</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21">
       <c r="A35">
         <v>0.06</v>
       </c>
@@ -2446,7 +4465,7 @@
         <v>6.0511990041751851</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21">
       <c r="A36">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2530,7 +4549,7 @@
         <v>7.2330550700676337</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21">
       <c r="A37">
         <v>0.08</v>
       </c>
@@ -2614,7 +4633,7 @@
         <v>8.6314021182394587</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21">
       <c r="A38">
         <v>0.09</v>
       </c>
@@ -2698,7 +4717,7 @@
         <v>10.283322509684954</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21">
       <c r="A39">
         <v>0.1</v>
       </c>
@@ -2782,7 +4801,7 @@
         <v>12.231818089682926</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21">
       <c r="A40">
         <v>0.11</v>
       </c>
@@ -2866,7 +4885,7 @@
         <v>14.526687452484959</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21">
       <c r="A41">
         <v>0.12</v>
       </c>
@@ -2950,7 +4969,7 @@
         <v>17.225523380848127</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21">
       <c r="A42">
         <v>0.13</v>
       </c>
@@ -3034,7 +5053,7 @@
         <v>20.39484560128027</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21">
       <c r="A43">
         <v>0.14000000000000001</v>
       </c>
@@ -3118,7 +5137,7 @@
         <v>24.111385740096527</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21">
       <c r="A44">
         <v>0.15</v>
       </c>
@@ -3202,118 +5221,118 @@
         <v>28.463543292080157</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="34.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" ht="34.5">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>5.0034722222222223</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <f>B47+B47</f>
         <v>10.006944444444445</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <f>C47+B47</f>
         <v>15.010416666666668</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <f>D47+$B$47</f>
         <v>20.013888888888889</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="2">
         <f t="shared" ref="F47:U47" si="4">E47+$B$47</f>
         <v>25.017361111111111</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="2">
         <f t="shared" si="4"/>
         <v>30.020833333333332</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="2">
         <f t="shared" si="4"/>
         <v>35.024305555555557</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="2">
         <f t="shared" si="4"/>
         <v>40.027777777777779</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="2">
         <f t="shared" si="4"/>
         <v>45.03125</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="2">
         <f t="shared" si="4"/>
         <v>50.034722222222221</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="2">
         <f t="shared" si="4"/>
         <v>55.038194444444443</v>
       </c>
-      <c r="M47" s="3">
+      <c r="M47" s="2">
         <f t="shared" si="4"/>
         <v>60.041666666666664</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="2">
         <f t="shared" si="4"/>
         <v>65.045138888888886</v>
       </c>
-      <c r="O47" s="3">
+      <c r="O47" s="2">
         <f t="shared" si="4"/>
         <v>70.048611111111114</v>
       </c>
-      <c r="P47" s="3">
+      <c r="P47" s="2">
         <f t="shared" si="4"/>
         <v>75.052083333333343</v>
       </c>
-      <c r="Q47" s="3">
+      <c r="Q47" s="2">
         <f t="shared" si="4"/>
         <v>80.055555555555571</v>
       </c>
-      <c r="R47" s="3">
+      <c r="R47" s="2">
         <f t="shared" si="4"/>
         <v>85.0590277777778</v>
       </c>
-      <c r="S47" s="3">
+      <c r="S47" s="2">
         <f t="shared" si="4"/>
         <v>90.062500000000028</v>
       </c>
-      <c r="T47" s="3">
+      <c r="T47" s="2">
         <f t="shared" si="4"/>
         <v>95.065972222222257</v>
       </c>
-      <c r="U47" s="3">
+      <c r="U47" s="2">
         <f t="shared" si="4"/>
         <v>100.06944444444449</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -3378,7 +5397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -3463,7 +5482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -3548,34 +5567,519 @@
         <v>2.1700637341075684</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
       <c r="A53">
         <v>1</v>
       </c>
+      <c r="B53">
+        <f>2*(1+((B$49*$A53)/100))</f>
+        <v>2.06</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ref="C53:U58" si="7">2*(1+((C$49*$A53)/100))</f>
+        <v>2.04</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="7"/>
+        <v>2.02</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="7"/>
+        <v>1.92</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="7"/>
+        <v>1.98</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="7"/>
+        <v>2.06</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="7"/>
+        <v>2.02</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="7"/>
+        <v>2.06</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="7"/>
+        <v>1.9</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="7"/>
+        <v>2.04</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="7"/>
+        <v>1.98</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="7"/>
+        <v>2.04</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="7"/>
+        <v>1.92</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="7"/>
+        <v>1.98</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="7"/>
+        <v>2.06</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="7"/>
+        <v>2.02</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="7"/>
+        <v>2.02</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="7"/>
+        <v>1.96</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="7"/>
+        <v>1.96</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="7"/>
+        <v>2.14</v>
+      </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21">
       <c r="A54">
-        <v>1.1000000000000001</v>
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <f t="shared" ref="B54:Q58" si="8">2*(1+((B$49*$A54)/100))</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="8"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="8"/>
+        <v>2.1</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="8"/>
+        <v>1.6</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="8"/>
+        <v>1.9</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="8"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="8"/>
+        <v>2.1</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="8"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="8"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="8"/>
+        <v>1.9</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="8"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="8"/>
+        <v>1.6</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="8"/>
+        <v>1.9</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="8"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="8"/>
+        <v>2.1</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="7"/>
+        <v>2.1</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="7"/>
+        <v>2.7</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21">
       <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="8"/>
+        <v>2.6</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="7"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="7"/>
         <v>1.2</v>
       </c>
+      <c r="F55">
+        <f t="shared" si="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="7"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="7"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="7"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="7"/>
+        <v>3.4</v>
+      </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21">
       <c r="A56">
-        <v>1.3</v>
+        <v>15</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="8"/>
+        <v>2.9</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="7"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="7"/>
+        <v>1.7</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="7"/>
+        <v>2.9</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="7"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="7"/>
+        <v>2.9</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="7"/>
+        <v>1.7</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="7"/>
+        <v>1.7</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="7"/>
+        <v>2.9</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="7"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="7"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="7"/>
+        <v>1.4</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="7"/>
+        <v>1.4</v>
+      </c>
+      <c r="U56">
+        <f t="shared" si="7"/>
+        <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21">
       <c r="A57">
-        <v>1.4</v>
+        <v>20</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="8"/>
+        <v>3.2</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="7"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="7"/>
+        <v>3.2</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="7"/>
+        <v>3.2</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="7"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="7"/>
+        <v>3.2</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="U57">
+        <f t="shared" si="7"/>
+        <v>4.8</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21">
       <c r="A58">
+        <v>25</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="8"/>
+        <v>3.5</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="7"/>
         <v>1.5</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="7"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U58">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -3598,4 +6102,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="58.5" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
final checkin of day
</commit_message>
<xml_diff>
--- a/beursbar_calculate_prices/simulation.xlsx
+++ b/beursbar_calculate_prices/simulation.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Personal\Visual Studio 2017\Projects\beursbar_calc_prices\beursbar_calculate_prices\"/>
@@ -176,11 +176,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -212,17 +212,74 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -325,17 +382,74 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -425,64 +539,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.06</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2.04</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.02</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1.92</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>1.98</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.06</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.02</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.06</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.04</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.98</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.04</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.92</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.98</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.06</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.02</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.96</c:v>
+                  <c:v>2.02</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.96</c:v>
+                  <c:v>2.04</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.14</c:v>
+                  <c:v>2.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,17 +612,74 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -598,64 +769,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.1</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>1.9</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.8</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.7</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,17 +842,74 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -771,64 +999,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>1.8</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.6</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.6</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.4</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,17 +1072,74 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -944,64 +1229,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.9</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2.6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>1.7</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.2999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.9</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.4</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.4</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1017,17 +1302,74 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -1117,64 +1459,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0.39999999999999991</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>1.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.39999999999999991</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.2</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.2</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.8</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1190,19 +1532,76 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:extLst>
@@ -1292,64 +1691,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.5</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1362,13 +1761,52 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:upBars>
+          <c:downBars>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:downBars>
+        </c:upDownBars>
         <c:smooth val="0"/>
         <c:axId val="463273928"/>
         <c:axId val="400039744"/>
@@ -1386,7 +1824,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -1394,6 +1832,7 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1438,6 +1877,7 @@
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1451,8 +1891,15 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1489,7 +1936,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1592,7 +2039,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="237">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1603,7 +2050,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1616,7 +2063,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -1624,6 +2071,7 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1649,7 +2097,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1693,7 +2141,7 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1708,7 +2156,7 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1725,17 +2173,17 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
+        <a:miter lim="800000"/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
@@ -1743,7 +2191,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1754,19 +2202,20 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1791,15 +2240,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1809,13 +2256,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
@@ -1836,14 +2283,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1855,14 +2301,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -1873,12 +2318,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1893,6 +2332,7 @@
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
+            <a:alpha val="32000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1907,14 +2347,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
+            <a:alpha val="32000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1926,14 +2366,10 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
+          <a:schemeClr val="tx1"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1945,14 +2381,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1989,11 +2424,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2004,14 +2448,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2021,11 +2464,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2037,12 +2480,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
+      <a:ln w="12700" cap="rnd"/>
     </cs:spPr>
   </cs:trendline>
   <cs:trendlineLabel>
@@ -2062,7 +2500,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2071,8 +2509,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2088,6 +2526,18 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2097,21 +2547,15 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr codeName="Chart2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2448,10 +2892,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5337,64 +5782,64 @@
         <v>8</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48">
         <v>6</v>
       </c>
       <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>6</v>
+      </c>
+      <c r="H48">
         <v>2</v>
       </c>
-      <c r="F48">
+      <c r="I48">
         <v>1</v>
-      </c>
-      <c r="G48">
-        <v>4</v>
-      </c>
-      <c r="H48">
-        <v>5</v>
-      </c>
-      <c r="I48">
-        <v>8</v>
       </c>
       <c r="J48">
         <v>3</v>
       </c>
       <c r="K48">
+        <v>6</v>
+      </c>
+      <c r="L48">
+        <v>7</v>
+      </c>
+      <c r="M48">
         <v>5</v>
       </c>
-      <c r="L48">
-        <v>4</v>
-      </c>
-      <c r="M48">
-        <v>6</v>
-      </c>
       <c r="N48">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O48">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P48">
         <v>4</v>
       </c>
       <c r="Q48">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R48">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S48">
         <v>4</v>
       </c>
       <c r="T48">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="U48">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -5403,67 +5848,67 @@
       </c>
       <c r="B49">
         <f>B48-0</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49">
         <f>C48-B48</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49">
         <f t="shared" ref="D49:U49" si="5">D48-C48</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49">
         <f t="shared" si="5"/>
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="F49">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="G49">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H49">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="I49">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="J49">
         <f t="shared" si="5"/>
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L49">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M49">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="N49">
         <f t="shared" si="5"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="O49">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="P49">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Q49">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="R49">
         <f t="shared" si="5"/>
@@ -5471,15 +5916,15 @@
       </c>
       <c r="S49">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="T49">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="U49">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -5488,83 +5933,83 @@
       </c>
       <c r="B50">
         <f>2*(1+((B$49*$A53)/100))</f>
-        <v>2.06</v>
+        <v>2.02</v>
       </c>
       <c r="C50">
         <f>B50*(1+(C49/100))</f>
-        <v>2.1012</v>
+        <v>2.0806</v>
       </c>
       <c r="D50">
         <f t="shared" ref="D50:U50" si="6">C50*(1+(D49/100))</f>
-        <v>2.1222119999999998</v>
+        <v>2.1222120000000002</v>
       </c>
       <c r="E50">
         <f t="shared" si="6"/>
-        <v>2.0373235199999997</v>
+        <v>2.1646562400000002</v>
       </c>
       <c r="F50">
         <f t="shared" si="6"/>
-        <v>2.0169502847999996</v>
+        <v>2.0780699904</v>
       </c>
       <c r="G50">
         <f t="shared" si="6"/>
-        <v>2.0774587933439999</v>
+        <v>2.1196313902080002</v>
       </c>
       <c r="H50">
         <f t="shared" si="6"/>
-        <v>2.0982333812774399</v>
+        <v>2.0348461345996802</v>
       </c>
       <c r="I50">
         <f t="shared" si="6"/>
-        <v>2.161180382715763</v>
+        <v>2.0144976732536835</v>
       </c>
       <c r="J50">
         <f>I50*(1+(J49/100))</f>
-        <v>2.0531213635799745</v>
+        <v>2.054787626718757</v>
       </c>
       <c r="K50">
         <f t="shared" si="6"/>
-        <v>2.0941837908515741</v>
+        <v>2.11643125552032</v>
       </c>
       <c r="L50">
         <f t="shared" si="6"/>
-        <v>2.0732419529430586</v>
+        <v>2.1375955680755232</v>
       </c>
       <c r="M50">
         <f t="shared" si="6"/>
-        <v>2.1147067920019196</v>
+        <v>2.0948436567140125</v>
       </c>
       <c r="N50">
         <f t="shared" si="6"/>
-        <v>2.0301185203218428</v>
+        <v>2.1786374029825732</v>
       </c>
       <c r="O50">
         <f t="shared" si="6"/>
-        <v>2.0098173351186244</v>
+        <v>2.0914919068632702</v>
       </c>
       <c r="P50">
         <f t="shared" si="6"/>
-        <v>2.0701118551721831</v>
+        <v>2.0705769877946376</v>
       </c>
       <c r="Q50">
         <f t="shared" si="6"/>
-        <v>2.0908129737239047</v>
+        <v>2.0291654480387447</v>
       </c>
       <c r="R50">
         <f t="shared" si="6"/>
-        <v>2.1117211034611438</v>
+        <v>2.0494571025191322</v>
       </c>
       <c r="S50">
         <f t="shared" si="6"/>
-        <v>2.069486681391921</v>
+        <v>2.0699516735443235</v>
       </c>
       <c r="T50">
         <f t="shared" si="6"/>
-        <v>2.0280969477640824</v>
+        <v>2.1113507070152102</v>
       </c>
       <c r="U50">
         <f t="shared" si="6"/>
-        <v>2.1700637341075684</v>
+        <v>2.1535777211555143</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -5578,83 +6023,83 @@
       </c>
       <c r="B53">
         <f>2*(1+((B$49*$A53)/100))</f>
-        <v>2.06</v>
+        <v>2.02</v>
       </c>
       <c r="C53">
         <f t="shared" ref="C53:U58" si="7">2*(1+((C$49*$A53)/100))</f>
+        <v>2.06</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="7"/>
         <v>2.04</v>
       </c>
-      <c r="D53">
+      <c r="E53">
+        <f t="shared" si="7"/>
+        <v>2.04</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="7"/>
+        <v>1.92</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="7"/>
+        <v>2.04</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="7"/>
+        <v>1.92</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="7"/>
+        <v>1.98</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="7"/>
+        <v>2.04</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="7"/>
+        <v>2.06</v>
+      </c>
+      <c r="L53">
         <f t="shared" si="7"/>
         <v>2.02</v>
       </c>
-      <c r="E53">
+      <c r="M53">
+        <f t="shared" si="7"/>
+        <v>1.96</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="7"/>
+        <v>2.08</v>
+      </c>
+      <c r="O53">
         <f t="shared" si="7"/>
         <v>1.92</v>
       </c>
-      <c r="F53">
+      <c r="P53">
         <f t="shared" si="7"/>
         <v>1.98</v>
       </c>
-      <c r="G53">
-        <f t="shared" si="7"/>
-        <v>2.06</v>
-      </c>
-      <c r="H53">
+      <c r="Q53">
+        <f t="shared" si="7"/>
+        <v>1.96</v>
+      </c>
+      <c r="R53">
         <f t="shared" si="7"/>
         <v>2.02</v>
       </c>
-      <c r="I53">
-        <f t="shared" si="7"/>
-        <v>2.06</v>
-      </c>
-      <c r="J53">
-        <f t="shared" si="7"/>
-        <v>1.9</v>
-      </c>
-      <c r="K53">
+      <c r="S53">
+        <f t="shared" si="7"/>
+        <v>2.02</v>
+      </c>
+      <c r="T53">
         <f t="shared" si="7"/>
         <v>2.04</v>
       </c>
-      <c r="L53">
-        <f t="shared" si="7"/>
-        <v>1.98</v>
-      </c>
-      <c r="M53">
+      <c r="U53">
         <f t="shared" si="7"/>
         <v>2.04</v>
-      </c>
-      <c r="N53">
-        <f t="shared" si="7"/>
-        <v>1.92</v>
-      </c>
-      <c r="O53">
-        <f t="shared" si="7"/>
-        <v>1.98</v>
-      </c>
-      <c r="P53">
-        <f t="shared" si="7"/>
-        <v>2.06</v>
-      </c>
-      <c r="Q53">
-        <f t="shared" si="7"/>
-        <v>2.02</v>
-      </c>
-      <c r="R53">
-        <f t="shared" si="7"/>
-        <v>2.02</v>
-      </c>
-      <c r="S53">
-        <f t="shared" si="7"/>
-        <v>1.96</v>
-      </c>
-      <c r="T53">
-        <f t="shared" si="7"/>
-        <v>1.96</v>
-      </c>
-      <c r="U53">
-        <f t="shared" si="7"/>
-        <v>2.14</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -5663,83 +6108,83 @@
       </c>
       <c r="B54">
         <f t="shared" ref="B54:Q58" si="8">2*(1+((B$49*$A54)/100))</f>
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C54">
         <f t="shared" si="8"/>
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D54">
         <f t="shared" si="8"/>
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E54">
         <f t="shared" si="8"/>
-        <v>1.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F54">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="G54">
         <f t="shared" si="8"/>
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H54">
         <f t="shared" si="8"/>
-        <v>2.1</v>
+        <v>1.6</v>
       </c>
       <c r="I54">
         <f t="shared" si="8"/>
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="J54">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K54">
         <f t="shared" si="8"/>
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L54">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="M54">
         <f t="shared" si="8"/>
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="N54">
         <f t="shared" si="8"/>
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="O54">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="P54">
         <f t="shared" si="8"/>
-        <v>2.2999999999999998</v>
+        <v>1.9</v>
       </c>
       <c r="Q54">
         <f t="shared" si="8"/>
+        <v>1.8</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="7"/>
         <v>2.1</v>
       </c>
-      <c r="R54">
+      <c r="S54">
         <f t="shared" si="7"/>
         <v>2.1</v>
       </c>
-      <c r="S54">
-        <f t="shared" si="7"/>
-        <v>1.8</v>
-      </c>
       <c r="T54">
         <f t="shared" si="7"/>
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="U54">
         <f t="shared" si="7"/>
-        <v>2.7</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -5748,83 +6193,83 @@
       </c>
       <c r="B55">
         <f t="shared" si="8"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="7"/>
         <v>2.6</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <f t="shared" si="7"/>
         <v>2.4</v>
       </c>
-      <c r="D55">
+      <c r="E55">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="L55">
         <f t="shared" si="7"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E55">
+      <c r="M55">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="O55">
         <f t="shared" si="7"/>
         <v>1.2</v>
       </c>
-      <c r="F55">
+      <c r="P55">
         <f t="shared" si="7"/>
         <v>1.8</v>
       </c>
-      <c r="G55">
-        <f t="shared" si="7"/>
-        <v>2.6</v>
-      </c>
-      <c r="H55">
+      <c r="Q55">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="R55">
         <f t="shared" si="7"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="7"/>
-        <v>2.6</v>
-      </c>
-      <c r="J55">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="K55">
+      <c r="S55">
+        <f t="shared" si="7"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T55">
         <f t="shared" si="7"/>
         <v>2.4</v>
       </c>
-      <c r="L55">
-        <f t="shared" si="7"/>
-        <v>1.8</v>
-      </c>
-      <c r="M55">
+      <c r="U55">
         <f t="shared" si="7"/>
         <v>2.4</v>
-      </c>
-      <c r="N55">
-        <f t="shared" si="7"/>
-        <v>1.2</v>
-      </c>
-      <c r="O55">
-        <f t="shared" si="7"/>
-        <v>1.8</v>
-      </c>
-      <c r="P55">
-        <f t="shared" si="7"/>
-        <v>2.6</v>
-      </c>
-      <c r="Q55">
-        <f t="shared" si="7"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="R55">
-        <f t="shared" si="7"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="S55">
-        <f t="shared" si="7"/>
-        <v>1.6</v>
-      </c>
-      <c r="T55">
-        <f t="shared" si="7"/>
-        <v>1.6</v>
-      </c>
-      <c r="U55">
-        <f t="shared" si="7"/>
-        <v>3.4</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -5833,83 +6278,83 @@
       </c>
       <c r="B56">
         <f t="shared" si="8"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="7"/>
         <v>2.9</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <f t="shared" si="7"/>
         <v>2.6</v>
       </c>
-      <c r="D56">
+      <c r="E56">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="7"/>
+        <v>1.7</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="7"/>
+        <v>2.6</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="7"/>
+        <v>2.9</v>
+      </c>
+      <c r="L56">
         <f t="shared" si="7"/>
         <v>2.2999999999999998</v>
       </c>
-      <c r="E56">
+      <c r="M56">
+        <f t="shared" si="7"/>
+        <v>1.4</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="7"/>
+        <v>3.2</v>
+      </c>
+      <c r="O56">
         <f t="shared" si="7"/>
         <v>0.8</v>
       </c>
-      <c r="F56">
+      <c r="P56">
         <f t="shared" si="7"/>
         <v>1.7</v>
       </c>
-      <c r="G56">
-        <f t="shared" si="7"/>
-        <v>2.9</v>
-      </c>
-      <c r="H56">
+      <c r="Q56">
+        <f t="shared" si="7"/>
+        <v>1.4</v>
+      </c>
+      <c r="R56">
         <f t="shared" si="7"/>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I56">
-        <f t="shared" si="7"/>
-        <v>2.9</v>
-      </c>
-      <c r="J56">
-        <f t="shared" si="7"/>
-        <v>0.5</v>
-      </c>
-      <c r="K56">
+      <c r="S56">
+        <f t="shared" si="7"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T56">
         <f t="shared" si="7"/>
         <v>2.6</v>
       </c>
-      <c r="L56">
-        <f t="shared" si="7"/>
-        <v>1.7</v>
-      </c>
-      <c r="M56">
+      <c r="U56">
         <f t="shared" si="7"/>
         <v>2.6</v>
-      </c>
-      <c r="N56">
-        <f t="shared" si="7"/>
-        <v>0.8</v>
-      </c>
-      <c r="O56">
-        <f t="shared" si="7"/>
-        <v>1.7</v>
-      </c>
-      <c r="P56">
-        <f t="shared" si="7"/>
-        <v>2.9</v>
-      </c>
-      <c r="Q56">
-        <f t="shared" si="7"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="R56">
-        <f t="shared" si="7"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="S56">
-        <f t="shared" si="7"/>
-        <v>1.4</v>
-      </c>
-      <c r="T56">
-        <f t="shared" si="7"/>
-        <v>1.4</v>
-      </c>
-      <c r="U56">
-        <f t="shared" si="7"/>
-        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -5918,83 +6363,83 @@
       </c>
       <c r="B57">
         <f t="shared" si="8"/>
+        <v>2.4</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="7"/>
         <v>3.2</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <f t="shared" si="7"/>
         <v>2.8</v>
       </c>
-      <c r="D57">
+      <c r="E57">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="7"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="7"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="7"/>
+        <v>1.6</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="7"/>
+        <v>3.2</v>
+      </c>
+      <c r="L57">
         <f t="shared" si="7"/>
         <v>2.4</v>
       </c>
-      <c r="E57">
+      <c r="M57">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="7"/>
+        <v>3.6</v>
+      </c>
+      <c r="O57">
         <f t="shared" si="7"/>
         <v>0.39999999999999991</v>
       </c>
-      <c r="F57">
+      <c r="P57">
         <f t="shared" si="7"/>
         <v>1.6</v>
       </c>
-      <c r="G57">
-        <f t="shared" si="7"/>
-        <v>3.2</v>
-      </c>
-      <c r="H57">
+      <c r="Q57">
+        <f t="shared" si="7"/>
+        <v>1.2</v>
+      </c>
+      <c r="R57">
         <f t="shared" si="7"/>
         <v>2.4</v>
       </c>
-      <c r="I57">
-        <f t="shared" si="7"/>
-        <v>3.2</v>
-      </c>
-      <c r="J57">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K57">
+      <c r="S57">
+        <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="T57">
         <f t="shared" si="7"/>
         <v>2.8</v>
       </c>
-      <c r="L57">
-        <f t="shared" si="7"/>
-        <v>1.6</v>
-      </c>
-      <c r="M57">
+      <c r="U57">
         <f t="shared" si="7"/>
         <v>2.8</v>
-      </c>
-      <c r="N57">
-        <f t="shared" si="7"/>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="O57">
-        <f t="shared" si="7"/>
-        <v>1.6</v>
-      </c>
-      <c r="P57">
-        <f t="shared" si="7"/>
-        <v>3.2</v>
-      </c>
-      <c r="Q57">
-        <f t="shared" si="7"/>
-        <v>2.4</v>
-      </c>
-      <c r="R57">
-        <f t="shared" si="7"/>
-        <v>2.4</v>
-      </c>
-      <c r="S57">
-        <f t="shared" si="7"/>
-        <v>1.2</v>
-      </c>
-      <c r="T57">
-        <f t="shared" si="7"/>
-        <v>1.2</v>
-      </c>
-      <c r="U57">
-        <f t="shared" si="7"/>
-        <v>4.8</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -6003,83 +6448,83 @@
       </c>
       <c r="B58">
         <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="D58">
+      <c r="E58">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="L58">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="E58">
+      <c r="M58">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="O58">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F58">
+      <c r="P58">
         <f t="shared" si="7"/>
         <v>1.5</v>
       </c>
-      <c r="G58">
-        <f t="shared" si="7"/>
-        <v>3.5</v>
-      </c>
-      <c r="H58">
+      <c r="Q58">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R58">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
-      <c r="I58">
-        <f t="shared" si="7"/>
-        <v>3.5</v>
-      </c>
-      <c r="J58">
-        <f t="shared" si="7"/>
-        <v>-0.5</v>
-      </c>
-      <c r="K58">
+      <c r="S58">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="T58">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L58">
-        <f t="shared" si="7"/>
-        <v>1.5</v>
-      </c>
-      <c r="M58">
+      <c r="U58">
         <f t="shared" si="7"/>
         <v>3</v>
-      </c>
-      <c r="N58">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="O58">
-        <f t="shared" si="7"/>
-        <v>1.5</v>
-      </c>
-      <c r="P58">
-        <f t="shared" si="7"/>
-        <v>3.5</v>
-      </c>
-      <c r="Q58">
-        <f t="shared" si="7"/>
-        <v>2.5</v>
-      </c>
-      <c r="R58">
-        <f t="shared" si="7"/>
-        <v>2.5</v>
-      </c>
-      <c r="S58">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="T58">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="U58">
-        <f t="shared" si="7"/>
-        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -6106,6 +6551,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>